<commit_message>
Sort TableDefinitions and changelog alphabetically
Add SOCP as option to Network -> v0.1.2
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioA" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioB" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ScenarioA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ScenarioB" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -594,7 +594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="00008080"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -665,7 +665,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.1</t>
+          <t>v0.1.2</t>
         </is>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="O7" s="9" t="inlineStr">
         <is>
-          <t>[DC-OPF,TP,SN]</t>
+          <t>[SOCP,DC-OPF,TP,SN]</t>
         </is>
       </c>
       <c r="P7" s="9" t="inlineStr">
@@ -2114,12 +2114,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="00008080"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.1</t>
+          <t>v0.1.2</t>
         </is>
       </c>
     </row>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="O7" s="9" t="inlineStr">
         <is>
-          <t>[DC-OPF,TP,SN]</t>
+          <t>[SOCP,DC-OPF,TP,SN]</t>
         </is>
       </c>
       <c r="P7" s="9" t="inlineStr">
@@ -3639,6 +3639,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>